<commit_message>
add dynamic feature function
</commit_message>
<xml_diff>
--- a/config/data_config.xlsx
+++ b/config/data_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sweeney/WorkSpace/ards/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC1527F-D53A-1D42-B487-94F5D4D1FA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56179BF-E5A3-1241-ADE7-447262209F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18220" yWindow="21600" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{1B0A151C-8596-714B-A1E6-0FD56CF5616C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19560" activeTab="1" xr2:uid="{1B0A151C-8596-714B-A1E6-0FD56CF5616C}"/>
   </bookViews>
   <sheets>
     <sheet name="diagnosis groupings" sheetId="1" r:id="rId1"/>
@@ -749,9 +749,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> [0,115]</t>
-  </si>
-  <si>
     <t>Base Excess</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -790,27 +787,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>GCS (eyes)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GCS (intub)</t>
-  </si>
-  <si>
-    <t>GCS (total)</t>
-  </si>
-  <si>
-    <t>GCS (motor)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GCS (unable)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GCS (verbal)</t>
-  </si>
-  <si>
     <t>Temperature</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1560,6 +1536,34 @@
   </si>
   <si>
     <t>Limit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0,115]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCS Eyes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCS Intub</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCS Total</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCS Motor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCS Unable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCS Verbal</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1736,6 +1740,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1744,9 +1751,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2087,209 +2091,209 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="3" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="3" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="11"/>
+      <c r="B13" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="3" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="11"/>
+      <c r="B15" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="3" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="11"/>
+      <c r="B16" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="3" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="11"/>
+      <c r="B17" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="3" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="11"/>
+      <c r="B18" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="11"/>
+      <c r="B19" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="3" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="11"/>
+      <c r="B20" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="11"/>
+      <c r="B21" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="3" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" s="11"/>
+      <c r="B22" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="3" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="3" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="11"/>
+      <c r="B24" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="3" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="11"/>
+      <c r="B25" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="3" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="11"/>
+      <c r="B26" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="14"/>
-      <c r="B20" s="3" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="11"/>
+      <c r="B27" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="3" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="11"/>
+      <c r="B28" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="3" t="s">
+    <row r="29" spans="1:2">
+      <c r="A29" s="11"/>
+      <c r="B29" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="3" t="s">
+    <row r="30" spans="1:2">
+      <c r="A30" s="11"/>
+      <c r="B30" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="3" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" s="11"/>
+      <c r="B31" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="14"/>
-      <c r="B25" s="3" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" s="11"/>
+      <c r="B32" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="3" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" s="11"/>
+      <c r="B33" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="3" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" s="11"/>
+      <c r="B34" s="3" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="14"/>
-      <c r="B31" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="14"/>
-      <c r="B32" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="14"/>
-      <c r="B33" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="14"/>
-      <c r="B34" s="3" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -2297,7 +2301,7 @@
         <v>8</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -2305,7 +2309,7 @@
         <v>9</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -2313,201 +2317,201 @@
         <v>10</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="11"/>
+      <c r="B39" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="11"/>
+      <c r="B40" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="11"/>
+      <c r="B41" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="11"/>
+      <c r="B42" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="11"/>
+      <c r="B43" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="11"/>
+      <c r="B44" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="3" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" s="11"/>
+      <c r="B45" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="14"/>
-      <c r="B39" s="3" t="s">
+    <row r="46" spans="1:2">
+      <c r="A46" s="11"/>
+      <c r="B46" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="14"/>
-      <c r="B40" s="3" t="s">
+    <row r="47" spans="1:2">
+      <c r="A47" s="11"/>
+      <c r="B47" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="14"/>
-      <c r="B41" s="3" t="s">
+    <row r="48" spans="1:2">
+      <c r="A48" s="11"/>
+      <c r="B48" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="3" t="s">
+    <row r="49" spans="1:2">
+      <c r="A49" s="11"/>
+      <c r="B49" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="14"/>
-      <c r="B43" s="3" t="s">
+    <row r="50" spans="1:2">
+      <c r="A50" s="11"/>
+      <c r="B50" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="3" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" s="11"/>
+      <c r="B51" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="14"/>
-      <c r="B45" s="3" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" s="11"/>
+      <c r="B52" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="14"/>
-      <c r="B46" s="3" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" s="11"/>
+      <c r="B53" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="14"/>
-      <c r="B47" s="3" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" s="11"/>
+      <c r="B54" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="14"/>
-      <c r="B48" s="3" t="s">
+    <row r="55" spans="1:2">
+      <c r="A55" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="3" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" s="11"/>
+      <c r="B56" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="14"/>
-      <c r="B50" s="3" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="11"/>
+      <c r="B57" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="14"/>
-      <c r="B51" s="3" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" s="11"/>
+      <c r="B58" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="14"/>
-      <c r="B52" s="3" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="11"/>
+      <c r="B59" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="14"/>
-      <c r="B53" s="3" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="11"/>
+      <c r="B60" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="14"/>
-      <c r="B54" s="3" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="11"/>
+      <c r="B61" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B55" s="3" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="14"/>
-      <c r="B56" s="3" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" s="11"/>
+      <c r="B63" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="14"/>
-      <c r="B57" s="3" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" s="11"/>
+      <c r="B64" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="14"/>
-      <c r="B58" s="3" t="s">
+    <row r="65" spans="1:2">
+      <c r="A65" s="11"/>
+      <c r="B65" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="14"/>
-      <c r="B59" s="3" t="s">
+    <row r="66" spans="1:2">
+      <c r="A66" s="11"/>
+      <c r="B66" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="14"/>
-      <c r="B60" s="3" t="s">
+    <row r="67" spans="1:2">
+      <c r="A67" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="14"/>
-      <c r="B61" s="3" t="s">
+    <row r="68" spans="1:2">
+      <c r="A68" s="11"/>
+      <c r="B68" s="3" t="s">
         <v>184</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="14"/>
-      <c r="B63" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="14"/>
-      <c r="B64" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="14"/>
-      <c r="B65" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="14"/>
-      <c r="B66" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="14"/>
-      <c r="B68" s="3" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -2515,73 +2519,73 @@
         <v>15</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="10"/>
       <c r="B70" s="4" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="10"/>
       <c r="B71" s="4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="10"/>
       <c r="B72" s="4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="10"/>
       <c r="B73" s="4" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="10"/>
       <c r="B74" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="10"/>
       <c r="B75" s="4" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="10"/>
       <c r="B76" s="4" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="10"/>
       <c r="B77" s="4" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="10"/>
       <c r="B78" s="4" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="10"/>
       <c r="B79" s="4" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="10"/>
       <c r="B80" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -2589,13 +2593,13 @@
         <v>16</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="10"/>
       <c r="B82" s="4" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -2603,73 +2607,73 @@
         <v>17</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="10"/>
       <c r="B84" s="4" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="10"/>
       <c r="B85" s="4" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="10"/>
       <c r="B86" s="4" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="10"/>
       <c r="B87" s="4" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="10"/>
       <c r="B88" s="4" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="10"/>
       <c r="B89" s="4" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="10"/>
       <c r="B90" s="4" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="10"/>
       <c r="B91" s="4" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="10"/>
       <c r="B92" s="4" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="10"/>
       <c r="B93" s="4" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="10"/>
       <c r="B94" s="4" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2677,13 +2681,13 @@
         <v>18</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="10"/>
       <c r="B96" s="4" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -2691,67 +2695,67 @@
         <v>19</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="10"/>
       <c r="B98" s="4" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="10"/>
       <c r="B99" s="4" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="10"/>
       <c r="B100" s="4" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="10"/>
       <c r="B101" s="4" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="10"/>
       <c r="B102" s="4" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="10"/>
       <c r="B103" s="4" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="10"/>
       <c r="B104" s="4" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="10"/>
       <c r="B105" s="4" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="10"/>
       <c r="B106" s="4" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="10"/>
       <c r="B107" s="4" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2759,49 +2763,49 @@
         <v>20</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="10"/>
       <c r="B109" s="4" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="10"/>
       <c r="B110" s="4" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="10"/>
       <c r="B111" s="4" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="10"/>
       <c r="B112" s="4" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="10"/>
       <c r="B113" s="4" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="10"/>
       <c r="B114" s="4" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="10"/>
       <c r="B115" s="4" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2809,37 +2813,37 @@
         <v>21</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="10"/>
       <c r="B117" s="4" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="10"/>
       <c r="B118" s="4" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="10"/>
       <c r="B119" s="4" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="10"/>
       <c r="B120" s="4" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="10"/>
       <c r="B121" s="4" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2847,103 +2851,103 @@
         <v>22</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="10"/>
       <c r="B123" s="4" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="10"/>
       <c r="B124" s="4" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="10"/>
       <c r="B125" s="4" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="10"/>
       <c r="B126" s="4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="10"/>
       <c r="B127" s="4" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="10"/>
       <c r="B128" s="4" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="10"/>
       <c r="B129" s="4" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="10"/>
       <c r="B130" s="4" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="10"/>
       <c r="B131" s="4" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="10"/>
       <c r="B132" s="4" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="10"/>
       <c r="B133" s="4" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="10"/>
       <c r="B134" s="4" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="10"/>
       <c r="B135" s="4" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="10"/>
       <c r="B136" s="4" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="10"/>
       <c r="B137" s="4" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="10"/>
       <c r="B138" s="4" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2951,43 +2955,43 @@
         <v>23</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="10"/>
       <c r="B140" s="4" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="10"/>
       <c r="B141" s="4" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="10"/>
       <c r="B142" s="4" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="10"/>
       <c r="B143" s="4" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="10"/>
       <c r="B144" s="4" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="10"/>
       <c r="B145" s="4" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2995,321 +2999,321 @@
         <v>24</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="10"/>
       <c r="B147" s="4" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="10"/>
       <c r="B148" s="4" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="10"/>
       <c r="B149" s="4" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="10"/>
       <c r="B150" s="4" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="10"/>
       <c r="B151" s="4" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="10"/>
       <c r="B152" s="4" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="10"/>
       <c r="B153" s="4" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="10"/>
       <c r="B154" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" s="13"/>
+      <c r="B156" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" s="13"/>
+      <c r="B157" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" s="13"/>
+      <c r="B158" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" s="13"/>
+      <c r="B159" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" s="13"/>
+      <c r="B160" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" s="13"/>
+      <c r="B161" s="4" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
-      <c r="A155" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B155" s="4" t="s">
+    <row r="162" spans="1:2">
+      <c r="A162" s="13"/>
+      <c r="B162" s="4" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
-      <c r="A156" s="12"/>
-      <c r="B156" s="4" t="s">
+    <row r="163" spans="1:2">
+      <c r="A163" s="13"/>
+      <c r="B163" s="4" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
-      <c r="A157" s="12"/>
-      <c r="B157" s="4" t="s">
+    <row r="164" spans="1:2">
+      <c r="A164" s="13"/>
+      <c r="B164" s="4" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
-      <c r="A158" s="12"/>
-      <c r="B158" s="4" t="s">
+    <row r="165" spans="1:2">
+      <c r="A165" s="13"/>
+      <c r="B165" s="4" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
-      <c r="A159" s="12"/>
-      <c r="B159" s="4" t="s">
+    <row r="166" spans="1:2">
+      <c r="A166" s="13"/>
+      <c r="B166" s="4" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
-      <c r="A160" s="12"/>
-      <c r="B160" s="4" t="s">
+    <row r="167" spans="1:2">
+      <c r="A167" s="13"/>
+      <c r="B167" s="4" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
-      <c r="A161" s="12"/>
-      <c r="B161" s="4" t="s">
+    <row r="168" spans="1:2">
+      <c r="A168" s="13"/>
+      <c r="B168" s="4" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
-      <c r="A162" s="12"/>
-      <c r="B162" s="4" t="s">
+    <row r="169" spans="1:2">
+      <c r="A169" s="13"/>
+      <c r="B169" s="4" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
-      <c r="A163" s="12"/>
-      <c r="B163" s="4" t="s">
+    <row r="170" spans="1:2">
+      <c r="A170" s="13"/>
+      <c r="B170" s="4" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
-      <c r="A164" s="12"/>
-      <c r="B164" s="4" t="s">
+    <row r="171" spans="1:2">
+      <c r="A171" s="13"/>
+      <c r="B171" s="4" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
-      <c r="A165" s="12"/>
-      <c r="B165" s="4" t="s">
+    <row r="172" spans="1:2">
+      <c r="A172" s="13"/>
+      <c r="B172" s="4" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
-      <c r="A166" s="12"/>
-      <c r="B166" s="4" t="s">
+    <row r="173" spans="1:2">
+      <c r="A173" s="13"/>
+      <c r="B173" s="4" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
-      <c r="A167" s="12"/>
-      <c r="B167" s="4" t="s">
+    <row r="174" spans="1:2">
+      <c r="A174" s="13"/>
+      <c r="B174" s="4" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
-      <c r="A168" s="12"/>
-      <c r="B168" s="4" t="s">
+    <row r="175" spans="1:2">
+      <c r="A175" s="13"/>
+      <c r="B175" s="4" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
-      <c r="A169" s="12"/>
-      <c r="B169" s="4" t="s">
+    <row r="176" spans="1:2">
+      <c r="A176" s="13"/>
+      <c r="B176" s="4" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
-      <c r="A170" s="12"/>
-      <c r="B170" s="4" t="s">
+    <row r="177" spans="1:2">
+      <c r="A177" s="13"/>
+      <c r="B177" s="4" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
-      <c r="A171" s="12"/>
-      <c r="B171" s="4" t="s">
+    <row r="178" spans="1:2">
+      <c r="A178" s="13"/>
+      <c r="B178" s="4" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
-      <c r="A172" s="12"/>
-      <c r="B172" s="4" t="s">
+    <row r="179" spans="1:2">
+      <c r="A179" s="13"/>
+      <c r="B179" s="4" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
-      <c r="A173" s="12"/>
-      <c r="B173" s="4" t="s">
+    <row r="180" spans="1:2">
+      <c r="A180" s="13"/>
+      <c r="B180" s="4" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
-      <c r="A174" s="12"/>
-      <c r="B174" s="4" t="s">
+    <row r="181" spans="1:2">
+      <c r="A181" s="13"/>
+      <c r="B181" s="4" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
-      <c r="A175" s="12"/>
-      <c r="B175" s="4" t="s">
+    <row r="182" spans="1:2">
+      <c r="A182" s="13"/>
+      <c r="B182" s="4" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
-      <c r="A176" s="12"/>
-      <c r="B176" s="4" t="s">
+    <row r="183" spans="1:2">
+      <c r="A183" s="13"/>
+      <c r="B183" s="4" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
-      <c r="A177" s="12"/>
-      <c r="B177" s="4" t="s">
+    <row r="184" spans="1:2">
+      <c r="A184" s="13"/>
+      <c r="B184" s="4" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
-      <c r="A178" s="12"/>
-      <c r="B178" s="4" t="s">
+    <row r="185" spans="1:2">
+      <c r="A185" s="13"/>
+      <c r="B185" s="4" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
-      <c r="A179" s="12"/>
-      <c r="B179" s="4" t="s">
+    <row r="186" spans="1:2">
+      <c r="A186" s="13"/>
+      <c r="B186" s="4" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
-      <c r="A180" s="12"/>
-      <c r="B180" s="4" t="s">
+    <row r="187" spans="1:2">
+      <c r="A187" s="13"/>
+      <c r="B187" s="4" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
-      <c r="A181" s="12"/>
-      <c r="B181" s="4" t="s">
+    <row r="188" spans="1:2">
+      <c r="A188" s="13"/>
+      <c r="B188" s="4" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
-      <c r="A182" s="12"/>
-      <c r="B182" s="4" t="s">
+    <row r="189" spans="1:2">
+      <c r="A189" s="13"/>
+      <c r="B189" s="4" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
-      <c r="A183" s="12"/>
-      <c r="B183" s="4" t="s">
+    <row r="190" spans="1:2">
+      <c r="A190" s="13"/>
+      <c r="B190" s="4" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
-      <c r="A184" s="12"/>
-      <c r="B184" s="4" t="s">
+    <row r="191" spans="1:2">
+      <c r="A191" s="13"/>
+      <c r="B191" s="4" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
-      <c r="A185" s="12"/>
-      <c r="B185" s="4" t="s">
+    <row r="192" spans="1:2">
+      <c r="A192" s="13"/>
+      <c r="B192" s="4" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
-      <c r="A186" s="12"/>
-      <c r="B186" s="4" t="s">
+    <row r="193" spans="1:2">
+      <c r="A193" s="13"/>
+      <c r="B193" s="4" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
-      <c r="A187" s="12"/>
-      <c r="B187" s="4" t="s">
+    <row r="194" spans="1:2">
+      <c r="A194" s="13"/>
+      <c r="B194" s="4" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
-      <c r="A188" s="12"/>
-      <c r="B188" s="4" t="s">
+    <row r="195" spans="1:2">
+      <c r="A195" s="13"/>
+      <c r="B195" s="4" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
-      <c r="A189" s="12"/>
-      <c r="B189" s="4" t="s">
+    <row r="196" spans="1:2">
+      <c r="A196" s="13"/>
+      <c r="B196" s="4" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
-      <c r="A190" s="12"/>
-      <c r="B190" s="4" t="s">
+    <row r="197" spans="1:2">
+      <c r="A197" s="13"/>
+      <c r="B197" s="4" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
-      <c r="A191" s="12"/>
-      <c r="B191" s="4" t="s">
+    <row r="198" spans="1:2">
+      <c r="A198" s="14"/>
+      <c r="B198" s="4" t="s">
         <v>314</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2">
-      <c r="A192" s="12"/>
-      <c r="B192" s="4" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2">
-      <c r="A193" s="12"/>
-      <c r="B193" s="4" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2">
-      <c r="A194" s="12"/>
-      <c r="B194" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2">
-      <c r="A195" s="12"/>
-      <c r="B195" s="4" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2">
-      <c r="A196" s="12"/>
-      <c r="B196" s="4" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2">
-      <c r="A197" s="12"/>
-      <c r="B197" s="4" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2">
-      <c r="A198" s="13"/>
-      <c r="B198" s="4" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -3317,71 +3321,80 @@
         <v>26</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" s="10"/>
       <c r="B200" s="4" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" s="10"/>
       <c r="B201" s="4" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" s="10"/>
       <c r="B202" s="4" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" s="10"/>
       <c r="B203" s="4" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" s="10"/>
       <c r="B204" s="4" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" s="10"/>
       <c r="B205" s="4" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" s="10"/>
       <c r="B206" s="4" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" s="10"/>
       <c r="B207" s="4" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="10"/>
       <c r="B208" s="4" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" s="10"/>
       <c r="B209" s="4" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A146:A154"/>
+    <mergeCell ref="A155:A198"/>
+    <mergeCell ref="A199:A209"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="A97:A107"/>
+    <mergeCell ref="A108:A115"/>
+    <mergeCell ref="A116:A121"/>
+    <mergeCell ref="A122:A138"/>
+    <mergeCell ref="A139:A145"/>
     <mergeCell ref="A83:A94"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
@@ -3394,15 +3407,6 @@
     <mergeCell ref="A67:A68"/>
     <mergeCell ref="A69:A80"/>
     <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A146:A154"/>
-    <mergeCell ref="A155:A198"/>
-    <mergeCell ref="A199:A209"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="A97:A107"/>
-    <mergeCell ref="A108:A115"/>
-    <mergeCell ref="A116:A121"/>
-    <mergeCell ref="A122:A138"/>
-    <mergeCell ref="A139:A145"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3413,9 +3417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE9C029-4B67-BC48-953D-ADD0B2B7E79D}">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -3425,10 +3427,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="B1" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18">
@@ -3449,18 +3451,18 @@
     </row>
     <row r="4" spans="1:2" ht="18">
       <c r="A4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18">
       <c r="A5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18">
@@ -3473,13 +3475,13 @@
     </row>
     <row r="7" spans="1:2" ht="18">
       <c r="A7" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="6"/>
     </row>
     <row r="8" spans="1:2" ht="18">
       <c r="A8" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="7"/>
     </row>
@@ -3504,7 +3506,7 @@
         <v>73</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>74</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18">
@@ -3533,21 +3535,21 @@
     </row>
     <row r="15" spans="1:2" ht="17">
       <c r="A15" s="8" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18">
       <c r="A16" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B16" s="6"/>
     </row>
     <row r="17" spans="1:2" ht="17">
       <c r="A17" s="8" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B17" s="6"/>
     </row>
@@ -3561,37 +3563,37 @@
     </row>
     <row r="19" spans="1:2" ht="18">
       <c r="A19" s="5" t="s">
-        <v>85</v>
+        <v>329</v>
       </c>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:2" ht="17">
-      <c r="A20" s="8" t="s">
-        <v>86</v>
+    <row r="20" spans="1:2" ht="18">
+      <c r="A20" s="5" t="s">
+        <v>330</v>
       </c>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:2" ht="17">
-      <c r="A21" s="8" t="s">
-        <v>88</v>
+    <row r="21" spans="1:2" ht="18">
+      <c r="A21" s="5" t="s">
+        <v>331</v>
       </c>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:2" ht="17">
-      <c r="A22" s="8" t="s">
-        <v>87</v>
+    <row r="22" spans="1:2" ht="18">
+      <c r="A22" s="5" t="s">
+        <v>332</v>
       </c>
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:2" ht="17">
-      <c r="A23" s="8" t="s">
-        <v>89</v>
+    <row r="23" spans="1:2" ht="18">
+      <c r="A23" s="5" t="s">
+        <v>333</v>
       </c>
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:2" ht="17">
-      <c r="A24" s="8" t="s">
-        <v>90</v>
+    <row r="24" spans="1:2" ht="18">
+      <c r="A24" s="5" t="s">
+        <v>334</v>
       </c>
       <c r="B24" s="6"/>
     </row>
@@ -3613,10 +3615,10 @@
     </row>
     <row r="27" spans="1:2" ht="17">
       <c r="A27" s="8" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18">
@@ -3629,26 +3631,26 @@
     </row>
     <row r="29" spans="1:2" ht="17">
       <c r="A29" s="9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17">
       <c r="A30" s="8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="17">
       <c r="A31" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18">
@@ -3669,34 +3671,34 @@
     </row>
     <row r="34" spans="1:2" ht="17">
       <c r="A34" s="8" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17">
       <c r="A35" s="9" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17">
       <c r="A36" s="9" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17">
       <c r="A37" s="9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18">
@@ -3725,34 +3727,34 @@
     </row>
     <row r="41" spans="1:2" ht="17">
       <c r="A41" s="8" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="17">
       <c r="A42" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18">
       <c r="A43" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17">
       <c r="A44" s="8" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18">
@@ -3773,7 +3775,7 @@
     </row>
     <row r="47" spans="1:2" ht="18">
       <c r="A47" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B47" s="7"/>
     </row>
@@ -3787,10 +3789,10 @@
     </row>
     <row r="49" spans="1:2" ht="17">
       <c r="A49" s="8" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18">
@@ -3811,7 +3813,7 @@
     </row>
     <row r="52" spans="1:2" ht="17">
       <c r="A52" s="8" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>46</v>
@@ -3819,34 +3821,34 @@
     </row>
     <row r="53" spans="1:2" ht="17">
       <c r="A53" s="9" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="17">
       <c r="A54" s="9" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="17">
       <c r="A55" s="9" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="17">
       <c r="A56" s="8" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="18">
@@ -3859,10 +3861,10 @@
     </row>
     <row r="58" spans="1:2" ht="17">
       <c r="A58" s="8" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="18">

</xml_diff>

<commit_message>
db feature names change
</commit_message>
<xml_diff>
--- a/config/data_config.xlsx
+++ b/config/data_config.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sweeney/WorkSpace/ards/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F58F9A0-ACCF-B64B-8E69-B70586CCAB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4658F5-535F-6D49-94BB-24F8CB63EDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19560" activeTab="1" xr2:uid="{1B0A151C-8596-714B-A1E6-0FD56CF5616C}"/>
+    <workbookView xWindow="-18220" yWindow="21600" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{1B0A151C-8596-714B-A1E6-0FD56CF5616C}"/>
   </bookViews>
   <sheets>
     <sheet name="diagnosis groupings" sheetId="1" r:id="rId1"/>
     <sheet name="dynamic features range" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -597,10 +597,6 @@
     <t>[0,70]</t>
   </si>
   <si>
-    <t>bilirubin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>[0,20]</t>
   </si>
   <si>
@@ -1576,6 +1572,10 @@
   </si>
   <si>
     <t>ionized calcium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>total bilirubin</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1756,8 +1756,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1767,15 +1776,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2116,209 +2116,209 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="3" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="13"/>
+      <c r="B6" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="3" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="13"/>
+      <c r="B8" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="3" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" s="13"/>
+      <c r="B9" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="3" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="13"/>
+      <c r="B10" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="3" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="13"/>
+      <c r="B11" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="3" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="13"/>
+      <c r="B13" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="3" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="13"/>
+      <c r="B15" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="3" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="13"/>
+      <c r="B16" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="3" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="3" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="13"/>
+      <c r="B18" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="3" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="13"/>
+      <c r="B19" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="3" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="13"/>
+      <c r="B20" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="14"/>
-      <c r="B20" s="3" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="13"/>
+      <c r="B21" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="3" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" s="13"/>
+      <c r="B22" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="3" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="13"/>
+      <c r="B23" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="3" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="13"/>
+      <c r="B24" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="3" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="13"/>
+      <c r="B25" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="14"/>
-      <c r="B25" s="3" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="13"/>
+      <c r="B26" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="3" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="13"/>
+      <c r="B27" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="3" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="13"/>
+      <c r="B28" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="3" t="s">
+    <row r="29" spans="1:2">
+      <c r="A29" s="13"/>
+      <c r="B29" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="3" t="s">
+    <row r="30" spans="1:2">
+      <c r="A30" s="13"/>
+      <c r="B30" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="3" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" s="13"/>
+      <c r="B31" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="14"/>
-      <c r="B31" s="3" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" s="13"/>
+      <c r="B32" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="14"/>
-      <c r="B32" s="3" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" s="13"/>
+      <c r="B33" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="14"/>
-      <c r="B33" s="3" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" s="13"/>
+      <c r="B34" s="3" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="14"/>
-      <c r="B34" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -2326,7 +2326,7 @@
         <v>8</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -2334,7 +2334,7 @@
         <v>9</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -2342,1075 +2342,1084 @@
         <v>10</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="3" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="13"/>
+      <c r="B39" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="14"/>
-      <c r="B39" s="3" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" s="13"/>
+      <c r="B40" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="14"/>
-      <c r="B40" s="3" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" s="13"/>
+      <c r="B41" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="14"/>
-      <c r="B41" s="3" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" s="13"/>
+      <c r="B42" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="3" t="s">
+    <row r="43" spans="1:2">
+      <c r="A43" s="13"/>
+      <c r="B43" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="14"/>
-      <c r="B43" s="3" t="s">
+    <row r="44" spans="1:2">
+      <c r="A44" s="13"/>
+      <c r="B44" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="3" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" s="13"/>
+      <c r="B45" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="14"/>
-      <c r="B45" s="3" t="s">
+    <row r="46" spans="1:2">
+      <c r="A46" s="13"/>
+      <c r="B46" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="14"/>
-      <c r="B46" s="3" t="s">
+    <row r="47" spans="1:2">
+      <c r="A47" s="13"/>
+      <c r="B47" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="14"/>
-      <c r="B47" s="3" t="s">
+    <row r="48" spans="1:2">
+      <c r="A48" s="13"/>
+      <c r="B48" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="14"/>
-      <c r="B48" s="3" t="s">
+    <row r="49" spans="1:2">
+      <c r="A49" s="13"/>
+      <c r="B49" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="3" t="s">
+    <row r="50" spans="1:2">
+      <c r="A50" s="13"/>
+      <c r="B50" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="14"/>
-      <c r="B50" s="3" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" s="13"/>
+      <c r="B51" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="14"/>
-      <c r="B51" s="3" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" s="13"/>
+      <c r="B52" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="14"/>
-      <c r="B52" s="3" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" s="13"/>
+      <c r="B53" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="14"/>
-      <c r="B53" s="3" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" s="13"/>
+      <c r="B54" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="14"/>
-      <c r="B54" s="3" t="s">
+    <row r="55" spans="1:2">
+      <c r="A55" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B55" s="3" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" s="13"/>
+      <c r="B56" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="14"/>
-      <c r="B56" s="3" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="13"/>
+      <c r="B57" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="14"/>
-      <c r="B57" s="3" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" s="13"/>
+      <c r="B58" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="14"/>
-      <c r="B58" s="3" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="13"/>
+      <c r="B59" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="14"/>
-      <c r="B59" s="3" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="13"/>
+      <c r="B60" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="14"/>
-      <c r="B60" s="3" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="13"/>
+      <c r="B61" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="14"/>
-      <c r="B61" s="3" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B62" s="3" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" s="13"/>
+      <c r="B63" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="14"/>
-      <c r="B63" s="3" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" s="13"/>
+      <c r="B64" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="14"/>
-      <c r="B64" s="3" t="s">
+    <row r="65" spans="1:2">
+      <c r="A65" s="13"/>
+      <c r="B65" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="14"/>
-      <c r="B65" s="3" t="s">
+    <row r="66" spans="1:2">
+      <c r="A66" s="13"/>
+      <c r="B66" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="14"/>
-      <c r="B66" s="3" t="s">
+    <row r="67" spans="1:2">
+      <c r="A67" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B67" s="3" t="s">
+    <row r="68" spans="1:2">
+      <c r="A68" s="13"/>
+      <c r="B68" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="14"/>
-      <c r="B68" s="3" t="s">
+    <row r="69" spans="1:2">
+      <c r="A69" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B69" s="4" t="s">
+    <row r="70" spans="1:2">
+      <c r="A70" s="12"/>
+      <c r="B70" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="10"/>
-      <c r="B70" s="4" t="s">
+    <row r="71" spans="1:2">
+      <c r="A71" s="12"/>
+      <c r="B71" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="10"/>
-      <c r="B71" s="4" t="s">
+    <row r="72" spans="1:2">
+      <c r="A72" s="12"/>
+      <c r="B72" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="10"/>
-      <c r="B72" s="4" t="s">
+    <row r="73" spans="1:2">
+      <c r="A73" s="12"/>
+      <c r="B73" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="10"/>
-      <c r="B73" s="4" t="s">
+    <row r="74" spans="1:2">
+      <c r="A74" s="12"/>
+      <c r="B74" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="10"/>
-      <c r="B74" s="4" t="s">
+    <row r="75" spans="1:2">
+      <c r="A75" s="12"/>
+      <c r="B75" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="10"/>
-      <c r="B75" s="4" t="s">
+    <row r="76" spans="1:2">
+      <c r="A76" s="12"/>
+      <c r="B76" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="10"/>
-      <c r="B76" s="4" t="s">
+    <row r="77" spans="1:2">
+      <c r="A77" s="12"/>
+      <c r="B77" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="10"/>
-      <c r="B77" s="4" t="s">
+    <row r="78" spans="1:2">
+      <c r="A78" s="12"/>
+      <c r="B78" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="10"/>
-      <c r="B78" s="4" t="s">
+    <row r="79" spans="1:2">
+      <c r="A79" s="12"/>
+      <c r="B79" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="10"/>
-      <c r="B79" s="4" t="s">
+    <row r="80" spans="1:2">
+      <c r="A80" s="12"/>
+      <c r="B80" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="10"/>
-      <c r="B80" s="4" t="s">
+    <row r="81" spans="1:2">
+      <c r="A81" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B81" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B81" s="4" t="s">
+    <row r="82" spans="1:2">
+      <c r="A82" s="12"/>
+      <c r="B82" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="10"/>
-      <c r="B82" s="4" t="s">
+    <row r="83" spans="1:2">
+      <c r="A83" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B83" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B83" s="4" t="s">
+    <row r="84" spans="1:2">
+      <c r="A84" s="12"/>
+      <c r="B84" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="10"/>
-      <c r="B84" s="4" t="s">
+    <row r="85" spans="1:2">
+      <c r="A85" s="12"/>
+      <c r="B85" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="10"/>
-      <c r="B85" s="4" t="s">
+    <row r="86" spans="1:2">
+      <c r="A86" s="12"/>
+      <c r="B86" s="4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="10"/>
-      <c r="B86" s="4" t="s">
+    <row r="87" spans="1:2">
+      <c r="A87" s="12"/>
+      <c r="B87" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="10"/>
-      <c r="B87" s="4" t="s">
+    <row r="88" spans="1:2">
+      <c r="A88" s="12"/>
+      <c r="B88" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="10"/>
-      <c r="B88" s="4" t="s">
+    <row r="89" spans="1:2">
+      <c r="A89" s="12"/>
+      <c r="B89" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="10"/>
-      <c r="B89" s="4" t="s">
+    <row r="90" spans="1:2">
+      <c r="A90" s="12"/>
+      <c r="B90" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="10"/>
-      <c r="B90" s="4" t="s">
+    <row r="91" spans="1:2">
+      <c r="A91" s="12"/>
+      <c r="B91" s="4" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="10"/>
-      <c r="B91" s="4" t="s">
+    <row r="92" spans="1:2">
+      <c r="A92" s="12"/>
+      <c r="B92" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="10"/>
-      <c r="B92" s="4" t="s">
+    <row r="93" spans="1:2">
+      <c r="A93" s="12"/>
+      <c r="B93" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="10"/>
-      <c r="B93" s="4" t="s">
+    <row r="94" spans="1:2">
+      <c r="A94" s="12"/>
+      <c r="B94" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="10"/>
-      <c r="B94" s="4" t="s">
+    <row r="95" spans="1:2">
+      <c r="A95" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B95" s="4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B95" s="4" t="s">
+    <row r="96" spans="1:2">
+      <c r="A96" s="12"/>
+      <c r="B96" s="4" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="10"/>
-      <c r="B96" s="4" t="s">
+    <row r="97" spans="1:2">
+      <c r="A97" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B97" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B97" s="4" t="s">
+    <row r="98" spans="1:2">
+      <c r="A98" s="12"/>
+      <c r="B98" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="10"/>
-      <c r="B98" s="4" t="s">
+    <row r="99" spans="1:2">
+      <c r="A99" s="12"/>
+      <c r="B99" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="10"/>
-      <c r="B99" s="4" t="s">
+    <row r="100" spans="1:2">
+      <c r="A100" s="12"/>
+      <c r="B100" s="4" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="10"/>
-      <c r="B100" s="4" t="s">
+    <row r="101" spans="1:2">
+      <c r="A101" s="12"/>
+      <c r="B101" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
-      <c r="A101" s="10"/>
-      <c r="B101" s="4" t="s">
+    <row r="102" spans="1:2">
+      <c r="A102" s="12"/>
+      <c r="B102" s="4" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="10"/>
-      <c r="B102" s="4" t="s">
+    <row r="103" spans="1:2">
+      <c r="A103" s="12"/>
+      <c r="B103" s="4" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
-      <c r="A103" s="10"/>
-      <c r="B103" s="4" t="s">
+    <row r="104" spans="1:2">
+      <c r="A104" s="12"/>
+      <c r="B104" s="4" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
-      <c r="A104" s="10"/>
-      <c r="B104" s="4" t="s">
+    <row r="105" spans="1:2">
+      <c r="A105" s="12"/>
+      <c r="B105" s="4" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
-      <c r="A105" s="10"/>
-      <c r="B105" s="4" t="s">
+    <row r="106" spans="1:2">
+      <c r="A106" s="12"/>
+      <c r="B106" s="4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
-      <c r="A106" s="10"/>
-      <c r="B106" s="4" t="s">
+    <row r="107" spans="1:2">
+      <c r="A107" s="12"/>
+      <c r="B107" s="4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
-      <c r="A107" s="10"/>
-      <c r="B107" s="4" t="s">
+    <row r="108" spans="1:2">
+      <c r="A108" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B108" s="4" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B108" s="4" t="s">
+    <row r="109" spans="1:2">
+      <c r="A109" s="12"/>
+      <c r="B109" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
-      <c r="A109" s="10"/>
-      <c r="B109" s="4" t="s">
+    <row r="110" spans="1:2">
+      <c r="A110" s="12"/>
+      <c r="B110" s="4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
-      <c r="A110" s="10"/>
-      <c r="B110" s="4" t="s">
+    <row r="111" spans="1:2">
+      <c r="A111" s="12"/>
+      <c r="B111" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
-      <c r="A111" s="10"/>
-      <c r="B111" s="4" t="s">
+    <row r="112" spans="1:2">
+      <c r="A112" s="12"/>
+      <c r="B112" s="4" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
-      <c r="A112" s="10"/>
-      <c r="B112" s="4" t="s">
+    <row r="113" spans="1:2">
+      <c r="A113" s="12"/>
+      <c r="B113" s="4" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
-      <c r="A113" s="10"/>
-      <c r="B113" s="4" t="s">
+    <row r="114" spans="1:2">
+      <c r="A114" s="12"/>
+      <c r="B114" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
-      <c r="A114" s="10"/>
-      <c r="B114" s="4" t="s">
+    <row r="115" spans="1:2">
+      <c r="A115" s="12"/>
+      <c r="B115" s="4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
-      <c r="A115" s="10"/>
-      <c r="B115" s="4" t="s">
+    <row r="116" spans="1:2">
+      <c r="A116" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B116" s="4" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
-      <c r="A116" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B116" s="4" t="s">
+    <row r="117" spans="1:2">
+      <c r="A117" s="12"/>
+      <c r="B117" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
-      <c r="A117" s="10"/>
-      <c r="B117" s="4" t="s">
+    <row r="118" spans="1:2">
+      <c r="A118" s="12"/>
+      <c r="B118" s="4" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
-      <c r="A118" s="10"/>
-      <c r="B118" s="4" t="s">
+    <row r="119" spans="1:2">
+      <c r="A119" s="12"/>
+      <c r="B119" s="4" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
-      <c r="A119" s="10"/>
-      <c r="B119" s="4" t="s">
+    <row r="120" spans="1:2">
+      <c r="A120" s="12"/>
+      <c r="B120" s="4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
-      <c r="A120" s="10"/>
-      <c r="B120" s="4" t="s">
+    <row r="121" spans="1:2">
+      <c r="A121" s="12"/>
+      <c r="B121" s="4" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
-      <c r="A121" s="10"/>
-      <c r="B121" s="4" t="s">
+    <row r="122" spans="1:2">
+      <c r="A122" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B122" s="4" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
-      <c r="A122" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B122" s="4" t="s">
+    <row r="123" spans="1:2">
+      <c r="A123" s="12"/>
+      <c r="B123" s="4" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
-      <c r="A123" s="10"/>
-      <c r="B123" s="4" t="s">
+    <row r="124" spans="1:2">
+      <c r="A124" s="12"/>
+      <c r="B124" s="4" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
-      <c r="A124" s="10"/>
-      <c r="B124" s="4" t="s">
+    <row r="125" spans="1:2">
+      <c r="A125" s="12"/>
+      <c r="B125" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
-      <c r="A125" s="10"/>
-      <c r="B125" s="4" t="s">
+    <row r="126" spans="1:2">
+      <c r="A126" s="12"/>
+      <c r="B126" s="4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
-      <c r="A126" s="10"/>
-      <c r="B126" s="4" t="s">
+    <row r="127" spans="1:2">
+      <c r="A127" s="12"/>
+      <c r="B127" s="4" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
-      <c r="A127" s="10"/>
-      <c r="B127" s="4" t="s">
+    <row r="128" spans="1:2">
+      <c r="A128" s="12"/>
+      <c r="B128" s="4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
-      <c r="A128" s="10"/>
-      <c r="B128" s="4" t="s">
+    <row r="129" spans="1:2">
+      <c r="A129" s="12"/>
+      <c r="B129" s="4" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
-      <c r="A129" s="10"/>
-      <c r="B129" s="4" t="s">
+    <row r="130" spans="1:2">
+      <c r="A130" s="12"/>
+      <c r="B130" s="4" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
-      <c r="A130" s="10"/>
-      <c r="B130" s="4" t="s">
+    <row r="131" spans="1:2">
+      <c r="A131" s="12"/>
+      <c r="B131" s="4" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
-      <c r="A131" s="10"/>
-      <c r="B131" s="4" t="s">
+    <row r="132" spans="1:2">
+      <c r="A132" s="12"/>
+      <c r="B132" s="4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
-      <c r="A132" s="10"/>
-      <c r="B132" s="4" t="s">
+    <row r="133" spans="1:2">
+      <c r="A133" s="12"/>
+      <c r="B133" s="4" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
-      <c r="A133" s="10"/>
-      <c r="B133" s="4" t="s">
+    <row r="134" spans="1:2">
+      <c r="A134" s="12"/>
+      <c r="B134" s="4" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
-      <c r="A134" s="10"/>
-      <c r="B134" s="4" t="s">
+    <row r="135" spans="1:2">
+      <c r="A135" s="12"/>
+      <c r="B135" s="4" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
-      <c r="A135" s="10"/>
-      <c r="B135" s="4" t="s">
+    <row r="136" spans="1:2">
+      <c r="A136" s="12"/>
+      <c r="B136" s="4" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
-      <c r="A136" s="10"/>
-      <c r="B136" s="4" t="s">
+    <row r="137" spans="1:2">
+      <c r="A137" s="12"/>
+      <c r="B137" s="4" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
-      <c r="A137" s="10"/>
-      <c r="B137" s="4" t="s">
+    <row r="138" spans="1:2">
+      <c r="A138" s="12"/>
+      <c r="B138" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
-      <c r="A138" s="10"/>
-      <c r="B138" s="4" t="s">
+    <row r="139" spans="1:2">
+      <c r="A139" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B139" s="4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
-      <c r="A139" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B139" s="4" t="s">
+    <row r="140" spans="1:2">
+      <c r="A140" s="12"/>
+      <c r="B140" s="4" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
-      <c r="A140" s="10"/>
-      <c r="B140" s="4" t="s">
+    <row r="141" spans="1:2">
+      <c r="A141" s="12"/>
+      <c r="B141" s="4" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
-      <c r="A141" s="10"/>
-      <c r="B141" s="4" t="s">
+    <row r="142" spans="1:2">
+      <c r="A142" s="12"/>
+      <c r="B142" s="4" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
-      <c r="A142" s="10"/>
-      <c r="B142" s="4" t="s">
+    <row r="143" spans="1:2">
+      <c r="A143" s="12"/>
+      <c r="B143" s="4" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
-      <c r="A143" s="10"/>
-      <c r="B143" s="4" t="s">
+    <row r="144" spans="1:2">
+      <c r="A144" s="12"/>
+      <c r="B144" s="4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
-      <c r="A144" s="10"/>
-      <c r="B144" s="4" t="s">
+    <row r="145" spans="1:2">
+      <c r="A145" s="12"/>
+      <c r="B145" s="4" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
-      <c r="A145" s="10"/>
-      <c r="B145" s="4" t="s">
+    <row r="146" spans="1:2">
+      <c r="A146" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B146" s="4" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
-      <c r="A146" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B146" s="4" t="s">
+    <row r="147" spans="1:2">
+      <c r="A147" s="12"/>
+      <c r="B147" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
-      <c r="A147" s="10"/>
-      <c r="B147" s="4" t="s">
+    <row r="148" spans="1:2">
+      <c r="A148" s="12"/>
+      <c r="B148" s="4" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
-      <c r="A148" s="10"/>
-      <c r="B148" s="4" t="s">
+    <row r="149" spans="1:2">
+      <c r="A149" s="12"/>
+      <c r="B149" s="4" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
-      <c r="A149" s="10"/>
-      <c r="B149" s="4" t="s">
+    <row r="150" spans="1:2">
+      <c r="A150" s="12"/>
+      <c r="B150" s="4" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
-      <c r="A150" s="10"/>
-      <c r="B150" s="4" t="s">
+    <row r="151" spans="1:2">
+      <c r="A151" s="12"/>
+      <c r="B151" s="4" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
-      <c r="A151" s="10"/>
-      <c r="B151" s="4" t="s">
+    <row r="152" spans="1:2">
+      <c r="A152" s="12"/>
+      <c r="B152" s="4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
-      <c r="A152" s="10"/>
-      <c r="B152" s="4" t="s">
+    <row r="153" spans="1:2">
+      <c r="A153" s="12"/>
+      <c r="B153" s="4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
-      <c r="A153" s="10"/>
-      <c r="B153" s="4" t="s">
+    <row r="154" spans="1:2">
+      <c r="A154" s="12"/>
+      <c r="B154" s="4" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
-      <c r="A154" s="10"/>
-      <c r="B154" s="4" t="s">
+    <row r="155" spans="1:2">
+      <c r="A155" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B155" s="4" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
-      <c r="A155" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B155" s="4" t="s">
+    <row r="156" spans="1:2">
+      <c r="A156" s="15"/>
+      <c r="B156" s="4" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
-      <c r="A156" s="12"/>
-      <c r="B156" s="4" t="s">
+    <row r="157" spans="1:2">
+      <c r="A157" s="15"/>
+      <c r="B157" s="4" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
-      <c r="A157" s="12"/>
-      <c r="B157" s="4" t="s">
+    <row r="158" spans="1:2">
+      <c r="A158" s="15"/>
+      <c r="B158" s="4" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
-      <c r="A158" s="12"/>
-      <c r="B158" s="4" t="s">
+    <row r="159" spans="1:2">
+      <c r="A159" s="15"/>
+      <c r="B159" s="4" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
-      <c r="A159" s="12"/>
-      <c r="B159" s="4" t="s">
+    <row r="160" spans="1:2">
+      <c r="A160" s="15"/>
+      <c r="B160" s="4" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
-      <c r="A160" s="12"/>
-      <c r="B160" s="4" t="s">
+    <row r="161" spans="1:2">
+      <c r="A161" s="15"/>
+      <c r="B161" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
-      <c r="A161" s="12"/>
-      <c r="B161" s="4" t="s">
+    <row r="162" spans="1:2">
+      <c r="A162" s="15"/>
+      <c r="B162" s="4" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
-      <c r="A162" s="12"/>
-      <c r="B162" s="4" t="s">
+    <row r="163" spans="1:2">
+      <c r="A163" s="15"/>
+      <c r="B163" s="4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
-      <c r="A163" s="12"/>
-      <c r="B163" s="4" t="s">
+    <row r="164" spans="1:2">
+      <c r="A164" s="15"/>
+      <c r="B164" s="4" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
-      <c r="A164" s="12"/>
-      <c r="B164" s="4" t="s">
+    <row r="165" spans="1:2">
+      <c r="A165" s="15"/>
+      <c r="B165" s="4" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
-      <c r="A165" s="12"/>
-      <c r="B165" s="4" t="s">
+    <row r="166" spans="1:2">
+      <c r="A166" s="15"/>
+      <c r="B166" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
-      <c r="A166" s="12"/>
-      <c r="B166" s="4" t="s">
+    <row r="167" spans="1:2">
+      <c r="A167" s="15"/>
+      <c r="B167" s="4" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
-      <c r="A167" s="12"/>
-      <c r="B167" s="4" t="s">
+    <row r="168" spans="1:2">
+      <c r="A168" s="15"/>
+      <c r="B168" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
-      <c r="A168" s="12"/>
-      <c r="B168" s="4" t="s">
+    <row r="169" spans="1:2">
+      <c r="A169" s="15"/>
+      <c r="B169" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
-      <c r="A169" s="12"/>
-      <c r="B169" s="4" t="s">
+    <row r="170" spans="1:2">
+      <c r="A170" s="15"/>
+      <c r="B170" s="4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
-      <c r="A170" s="12"/>
-      <c r="B170" s="4" t="s">
+    <row r="171" spans="1:2">
+      <c r="A171" s="15"/>
+      <c r="B171" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
-      <c r="A171" s="12"/>
-      <c r="B171" s="4" t="s">
+    <row r="172" spans="1:2">
+      <c r="A172" s="15"/>
+      <c r="B172" s="4" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
-      <c r="A172" s="12"/>
-      <c r="B172" s="4" t="s">
+    <row r="173" spans="1:2">
+      <c r="A173" s="15"/>
+      <c r="B173" s="4" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
-      <c r="A173" s="12"/>
-      <c r="B173" s="4" t="s">
+    <row r="174" spans="1:2">
+      <c r="A174" s="15"/>
+      <c r="B174" s="4" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
-      <c r="A174" s="12"/>
-      <c r="B174" s="4" t="s">
+    <row r="175" spans="1:2">
+      <c r="A175" s="15"/>
+      <c r="B175" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
-      <c r="A175" s="12"/>
-      <c r="B175" s="4" t="s">
+    <row r="176" spans="1:2">
+      <c r="A176" s="15"/>
+      <c r="B176" s="4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
-      <c r="A176" s="12"/>
-      <c r="B176" s="4" t="s">
+    <row r="177" spans="1:2">
+      <c r="A177" s="15"/>
+      <c r="B177" s="4" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
-      <c r="A177" s="12"/>
-      <c r="B177" s="4" t="s">
+    <row r="178" spans="1:2">
+      <c r="A178" s="15"/>
+      <c r="B178" s="4" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
-      <c r="A178" s="12"/>
-      <c r="B178" s="4" t="s">
+    <row r="179" spans="1:2">
+      <c r="A179" s="15"/>
+      <c r="B179" s="4" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
-      <c r="A179" s="12"/>
-      <c r="B179" s="4" t="s">
+    <row r="180" spans="1:2">
+      <c r="A180" s="15"/>
+      <c r="B180" s="4" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
-      <c r="A180" s="12"/>
-      <c r="B180" s="4" t="s">
+    <row r="181" spans="1:2">
+      <c r="A181" s="15"/>
+      <c r="B181" s="4" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
-      <c r="A181" s="12"/>
-      <c r="B181" s="4" t="s">
+    <row r="182" spans="1:2">
+      <c r="A182" s="15"/>
+      <c r="B182" s="4" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
-      <c r="A182" s="12"/>
-      <c r="B182" s="4" t="s">
+    <row r="183" spans="1:2">
+      <c r="A183" s="15"/>
+      <c r="B183" s="4" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
-      <c r="A183" s="12"/>
-      <c r="B183" s="4" t="s">
+    <row r="184" spans="1:2">
+      <c r="A184" s="15"/>
+      <c r="B184" s="4" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
-      <c r="A184" s="12"/>
-      <c r="B184" s="4" t="s">
+    <row r="185" spans="1:2">
+      <c r="A185" s="15"/>
+      <c r="B185" s="4" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
-      <c r="A185" s="12"/>
-      <c r="B185" s="4" t="s">
+    <row r="186" spans="1:2">
+      <c r="A186" s="15"/>
+      <c r="B186" s="4" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
-      <c r="A186" s="12"/>
-      <c r="B186" s="4" t="s">
+    <row r="187" spans="1:2">
+      <c r="A187" s="15"/>
+      <c r="B187" s="4" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
-      <c r="A187" s="12"/>
-      <c r="B187" s="4" t="s">
+    <row r="188" spans="1:2">
+      <c r="A188" s="15"/>
+      <c r="B188" s="4" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
-      <c r="A188" s="12"/>
-      <c r="B188" s="4" t="s">
+    <row r="189" spans="1:2">
+      <c r="A189" s="15"/>
+      <c r="B189" s="4" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
-      <c r="A189" s="12"/>
-      <c r="B189" s="4" t="s">
+    <row r="190" spans="1:2">
+      <c r="A190" s="15"/>
+      <c r="B190" s="4" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
-      <c r="A190" s="12"/>
-      <c r="B190" s="4" t="s">
+    <row r="191" spans="1:2">
+      <c r="A191" s="15"/>
+      <c r="B191" s="4" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
-      <c r="A191" s="12"/>
-      <c r="B191" s="4" t="s">
+    <row r="192" spans="1:2">
+      <c r="A192" s="15"/>
+      <c r="B192" s="4" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
-      <c r="A192" s="12"/>
-      <c r="B192" s="4" t="s">
+    <row r="193" spans="1:2">
+      <c r="A193" s="15"/>
+      <c r="B193" s="4" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
-      <c r="A193" s="12"/>
-      <c r="B193" s="4" t="s">
+    <row r="194" spans="1:2">
+      <c r="A194" s="15"/>
+      <c r="B194" s="4" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
-      <c r="A194" s="12"/>
-      <c r="B194" s="4" t="s">
+    <row r="195" spans="1:2">
+      <c r="A195" s="15"/>
+      <c r="B195" s="4" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
-      <c r="A195" s="12"/>
-      <c r="B195" s="4" t="s">
+    <row r="196" spans="1:2">
+      <c r="A196" s="15"/>
+      <c r="B196" s="4" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
-      <c r="A196" s="12"/>
-      <c r="B196" s="4" t="s">
+    <row r="197" spans="1:2">
+      <c r="A197" s="15"/>
+      <c r="B197" s="4" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
-      <c r="A197" s="12"/>
-      <c r="B197" s="4" t="s">
+    <row r="198" spans="1:2">
+      <c r="A198" s="16"/>
+      <c r="B198" s="4" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
-      <c r="A198" s="13"/>
-      <c r="B198" s="4" t="s">
+    <row r="199" spans="1:2">
+      <c r="A199" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B199" s="4" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
-      <c r="A199" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B199" s="4" t="s">
+    <row r="200" spans="1:2">
+      <c r="A200" s="12"/>
+      <c r="B200" s="4" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
-      <c r="A200" s="10"/>
-      <c r="B200" s="4" t="s">
+    <row r="201" spans="1:2">
+      <c r="A201" s="12"/>
+      <c r="B201" s="4" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
-      <c r="A201" s="10"/>
-      <c r="B201" s="4" t="s">
+    <row r="202" spans="1:2">
+      <c r="A202" s="12"/>
+      <c r="B202" s="4" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
-      <c r="A202" s="10"/>
-      <c r="B202" s="4" t="s">
+    <row r="203" spans="1:2">
+      <c r="A203" s="12"/>
+      <c r="B203" s="4" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
-      <c r="A203" s="10"/>
-      <c r="B203" s="4" t="s">
+    <row r="204" spans="1:2">
+      <c r="A204" s="12"/>
+      <c r="B204" s="4" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
-      <c r="A204" s="10"/>
-      <c r="B204" s="4" t="s">
+    <row r="205" spans="1:2">
+      <c r="A205" s="12"/>
+      <c r="B205" s="4" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
-      <c r="A205" s="10"/>
-      <c r="B205" s="4" t="s">
+    <row r="206" spans="1:2">
+      <c r="A206" s="12"/>
+      <c r="B206" s="4" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
-      <c r="A206" s="10"/>
-      <c r="B206" s="4" t="s">
+    <row r="207" spans="1:2">
+      <c r="A207" s="12"/>
+      <c r="B207" s="4" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
-      <c r="A207" s="10"/>
-      <c r="B207" s="4" t="s">
+    <row r="208" spans="1:2">
+      <c r="A208" s="12"/>
+      <c r="B208" s="4" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
-      <c r="A208" s="10"/>
-      <c r="B208" s="4" t="s">
+    <row r="209" spans="1:2">
+      <c r="A209" s="12"/>
+      <c r="B209" s="4" t="s">
         <v>307</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2">
-      <c r="A209" s="10"/>
-      <c r="B209" s="4" t="s">
-        <v>308</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A146:A154"/>
+    <mergeCell ref="A155:A198"/>
+    <mergeCell ref="A199:A209"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="A97:A107"/>
+    <mergeCell ref="A108:A115"/>
+    <mergeCell ref="A116:A121"/>
+    <mergeCell ref="A122:A138"/>
+    <mergeCell ref="A139:A145"/>
     <mergeCell ref="A83:A94"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
@@ -3423,15 +3432,6 @@
     <mergeCell ref="A67:A68"/>
     <mergeCell ref="A69:A80"/>
     <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A146:A154"/>
-    <mergeCell ref="A155:A198"/>
-    <mergeCell ref="A199:A209"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="A97:A107"/>
-    <mergeCell ref="A108:A115"/>
-    <mergeCell ref="A116:A121"/>
-    <mergeCell ref="A122:A138"/>
-    <mergeCell ref="A139:A145"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3443,7 +3443,7 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E68"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3455,10 +3455,10 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B1" t="s">
         <v>309</v>
-      </c>
-      <c r="B1" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18">
@@ -3468,38 +3468,38 @@
       <c r="B2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" ht="18">
       <c r="A3" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+        <v>331</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5" ht="18">
       <c r="A4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5" ht="18">
       <c r="A5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5" ht="18">
       <c r="A6" s="5" t="s">
@@ -3508,524 +3508,524 @@
       <c r="B6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5" ht="18">
       <c r="A7" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:5" ht="18">
       <c r="A8" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="7"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:5" ht="18">
       <c r="A9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:5" ht="18">
       <c r="A10" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:5" ht="18">
       <c r="A11" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
+        <v>310</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:5" ht="18">
       <c r="A12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:5" ht="18">
       <c r="A13" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
+        <v>329</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" ht="18">
       <c r="A14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5" ht="17">
       <c r="A15" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
+        <v>330</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:5" ht="18">
       <c r="A16" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" s="6"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" ht="17">
       <c r="A17" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B17" s="6"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:5" ht="18">
       <c r="A18" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
+        <v>333</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" ht="18">
       <c r="A19" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B19" s="6"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
     </row>
     <row r="20" spans="1:5" ht="18">
       <c r="A20" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B20" s="6"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" ht="18">
       <c r="A21" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B21" s="6"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" spans="1:5" ht="18">
       <c r="A22" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B22" s="6"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
     </row>
     <row r="23" spans="1:5" ht="18">
       <c r="A23" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B23" s="6"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
     </row>
     <row r="24" spans="1:5" ht="18">
       <c r="A24" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B24" s="6"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:5" ht="18">
       <c r="A25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
     </row>
     <row r="26" spans="1:5" ht="18">
       <c r="A26" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
     </row>
     <row r="27" spans="1:5" ht="17">
       <c r="A27" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
+        <v>95</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
     </row>
     <row r="28" spans="1:5" ht="18">
       <c r="A28" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:5" ht="17">
       <c r="A29" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
+        <v>98</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:5" ht="17">
       <c r="A30" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
+        <v>99</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
     </row>
     <row r="31" spans="1:5" ht="17">
       <c r="A31" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
+        <v>97</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
     </row>
     <row r="32" spans="1:5" ht="18">
       <c r="A32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
     </row>
     <row r="33" spans="1:5" ht="18">
       <c r="A33" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
+        <v>329</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
     </row>
     <row r="34" spans="1:5" ht="17">
       <c r="A34" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:5" ht="17">
       <c r="A35" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
+        <v>94</v>
+      </c>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
     </row>
     <row r="36" spans="1:5" ht="17">
       <c r="A36" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
+        <v>94</v>
+      </c>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
     </row>
     <row r="37" spans="1:5" ht="17">
       <c r="A37" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
+        <v>93</v>
+      </c>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
     </row>
     <row r="38" spans="1:5" ht="18">
       <c r="A38" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="18">
       <c r="A39" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18">
       <c r="A40" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="17">
       <c r="A41" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="17">
       <c r="A42" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="18">
       <c r="A43" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="17">
       <c r="A44" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18">
       <c r="A45" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18">
       <c r="A46" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18">
       <c r="A47" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B47" s="7"/>
     </row>
     <row r="48" spans="1:5" ht="18">
       <c r="A48" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="17">
       <c r="A49" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18">
       <c r="A50" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18">
       <c r="A51" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="17">
       <c r="A52" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="17">
       <c r="A53" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="17">
       <c r="A54" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="17">
       <c r="A55" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="17">
       <c r="A56" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B56" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="18">
       <c r="A57" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="17">
       <c r="A58" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18">
       <c r="A59" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B59" s="6" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="D60" s="16"/>
-      <c r="E60" s="16"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
     </row>
     <row r="65" spans="4:5">
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
     </row>
     <row r="66" spans="4:5">
-      <c r="D66" s="16"/>
-      <c r="E66" s="16"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
     </row>
     <row r="67" spans="4:5">
-      <c r="D67" s="16"/>
-      <c r="E67" s="16"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
     </row>
     <row r="68" spans="4:5">
-      <c r="D68" s="16"/>
-      <c r="E68" s="16"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
     </row>
     <row r="69" spans="4:5">
-      <c r="D69" s="16"/>
-      <c r="E69" s="16"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
     </row>
     <row r="70" spans="4:5">
-      <c r="D70" s="16"/>
-      <c r="E70" s="16"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
     </row>
     <row r="71" spans="4:5">
-      <c r="D71" s="16"/>
-      <c r="E71" s="16"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
     </row>
     <row r="72" spans="4:5">
-      <c r="D72" s="16"/>
-      <c r="E72" s="16"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:E77">

</xml_diff>

<commit_message>
add calculate of pf and rectify name bugs
</commit_message>
<xml_diff>
--- a/config/data_config.xlsx
+++ b/config/data_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sweeney/WorkSpace/ards/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7224BD4F-C060-1049-AFC9-2F41C358887A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89853E5-912F-8948-9D9B-17844DEFA55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18220" yWindow="21600" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{1B0A151C-8596-714B-A1E6-0FD56CF5616C}"/>
   </bookViews>
@@ -772,10 +772,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Respiration Rate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>[1,40]</t>
   </si>
   <si>
@@ -1576,6 +1572,10 @@
   </si>
   <si>
     <t>magnesium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Respiratory Rate</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2127,7 +2127,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2135,13 +2135,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="13"/>
       <c r="B4" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2149,13 +2149,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="13"/>
       <c r="B6" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2163,31 +2163,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="13"/>
       <c r="B8" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="13"/>
       <c r="B9" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="13"/>
       <c r="B10" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="13"/>
       <c r="B11" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2195,13 +2195,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="13"/>
       <c r="B13" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2209,127 +2209,127 @@
         <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="13"/>
       <c r="B15" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="13"/>
       <c r="B16" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="13"/>
       <c r="B17" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="13"/>
       <c r="B18" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="13"/>
       <c r="B19" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="13"/>
       <c r="B20" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="13"/>
       <c r="B21" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="13"/>
       <c r="B22" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="13"/>
       <c r="B23" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="13"/>
       <c r="B24" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="13"/>
       <c r="B25" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="13"/>
       <c r="B26" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="13"/>
       <c r="B27" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="13"/>
       <c r="B28" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="13"/>
       <c r="B29" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="13"/>
       <c r="B30" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="13"/>
       <c r="B31" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="13"/>
       <c r="B32" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="13"/>
       <c r="B33" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="13"/>
       <c r="B34" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -2337,7 +2337,7 @@
         <v>8</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -2345,7 +2345,7 @@
         <v>9</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -2353,7 +2353,7 @@
         <v>10</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -2361,103 +2361,103 @@
         <v>11</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="13"/>
       <c r="B39" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="13"/>
       <c r="B40" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="13"/>
       <c r="B41" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="13"/>
       <c r="B42" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="13"/>
       <c r="B43" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="13"/>
       <c r="B44" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="13"/>
       <c r="B45" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="13"/>
       <c r="B46" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="13"/>
       <c r="B47" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="13"/>
       <c r="B48" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="13"/>
       <c r="B49" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="13"/>
       <c r="B50" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="13"/>
       <c r="B51" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="13"/>
       <c r="B52" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="13"/>
       <c r="B53" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="13"/>
       <c r="B54" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -2465,43 +2465,43 @@
         <v>12</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="13"/>
       <c r="B56" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="13"/>
       <c r="B57" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="13"/>
       <c r="B58" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="13"/>
       <c r="B59" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="13"/>
       <c r="B60" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="13"/>
       <c r="B61" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -2509,31 +2509,31 @@
         <v>13</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="13"/>
       <c r="B63" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="13"/>
       <c r="B64" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="13"/>
       <c r="B65" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="13"/>
       <c r="B66" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -2541,13 +2541,13 @@
         <v>14</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="13"/>
       <c r="B68" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -2555,73 +2555,73 @@
         <v>15</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="12"/>
       <c r="B70" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="12"/>
       <c r="B71" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="12"/>
       <c r="B72" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="12"/>
       <c r="B73" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="12"/>
       <c r="B74" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="12"/>
       <c r="B75" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="12"/>
       <c r="B76" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="12"/>
       <c r="B77" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="12"/>
       <c r="B78" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="12"/>
       <c r="B79" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="12"/>
       <c r="B80" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -2629,13 +2629,13 @@
         <v>16</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="12"/>
       <c r="B82" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -2643,73 +2643,73 @@
         <v>17</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="12"/>
       <c r="B84" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="12"/>
       <c r="B85" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="12"/>
       <c r="B86" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="12"/>
       <c r="B87" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="12"/>
       <c r="B88" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="12"/>
       <c r="B89" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="12"/>
       <c r="B90" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="12"/>
       <c r="B91" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="12"/>
       <c r="B92" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="12"/>
       <c r="B93" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="12"/>
       <c r="B94" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2717,13 +2717,13 @@
         <v>18</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="12"/>
       <c r="B96" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -2731,67 +2731,67 @@
         <v>19</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="12"/>
       <c r="B98" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="12"/>
       <c r="B99" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="12"/>
       <c r="B100" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="12"/>
       <c r="B101" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="12"/>
       <c r="B102" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="12"/>
       <c r="B103" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="12"/>
       <c r="B104" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="12"/>
       <c r="B105" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="12"/>
       <c r="B106" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="12"/>
       <c r="B107" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2799,49 +2799,49 @@
         <v>20</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="12"/>
       <c r="B109" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="12"/>
       <c r="B110" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="12"/>
       <c r="B111" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="12"/>
       <c r="B112" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="12"/>
       <c r="B113" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="12"/>
       <c r="B114" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="12"/>
       <c r="B115" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2849,37 +2849,37 @@
         <v>21</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="12"/>
       <c r="B117" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="12"/>
       <c r="B118" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="12"/>
       <c r="B119" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="12"/>
       <c r="B120" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="12"/>
       <c r="B121" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2887,103 +2887,103 @@
         <v>22</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="12"/>
       <c r="B123" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="12"/>
       <c r="B124" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="12"/>
       <c r="B125" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="12"/>
       <c r="B126" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="12"/>
       <c r="B127" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="12"/>
       <c r="B128" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="12"/>
       <c r="B129" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="12"/>
       <c r="B130" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="12"/>
       <c r="B131" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="12"/>
       <c r="B132" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="12"/>
       <c r="B133" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="12"/>
       <c r="B134" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="12"/>
       <c r="B135" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="12"/>
       <c r="B136" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="12"/>
       <c r="B137" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="12"/>
       <c r="B138" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2991,43 +2991,43 @@
         <v>23</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="12"/>
       <c r="B140" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="12"/>
       <c r="B141" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="12"/>
       <c r="B142" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="12"/>
       <c r="B143" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="12"/>
       <c r="B144" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="12"/>
       <c r="B145" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -3035,55 +3035,55 @@
         <v>24</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="12"/>
       <c r="B147" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="12"/>
       <c r="B148" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="12"/>
       <c r="B149" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="12"/>
       <c r="B150" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="12"/>
       <c r="B151" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="12"/>
       <c r="B152" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="12"/>
       <c r="B153" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="12"/>
       <c r="B154" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -3091,265 +3091,265 @@
         <v>25</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="15"/>
       <c r="B156" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="15"/>
       <c r="B157" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="15"/>
       <c r="B158" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="15"/>
       <c r="B159" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="15"/>
       <c r="B160" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="15"/>
       <c r="B161" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="15"/>
       <c r="B162" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="15"/>
       <c r="B163" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="15"/>
       <c r="B164" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="15"/>
       <c r="B165" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="15"/>
       <c r="B166" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" s="15"/>
       <c r="B167" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="15"/>
       <c r="B168" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="15"/>
       <c r="B169" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="15"/>
       <c r="B170" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="15"/>
       <c r="B171" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" s="15"/>
       <c r="B172" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="15"/>
       <c r="B173" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="15"/>
       <c r="B174" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="15"/>
       <c r="B175" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="15"/>
       <c r="B176" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" s="15"/>
       <c r="B177" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="15"/>
       <c r="B178" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" s="15"/>
       <c r="B179" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" s="15"/>
       <c r="B180" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="15"/>
       <c r="B181" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" s="15"/>
       <c r="B182" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="15"/>
       <c r="B183" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" s="15"/>
       <c r="B184" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="15"/>
       <c r="B185" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="15"/>
       <c r="B186" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="15"/>
       <c r="B187" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" s="15"/>
       <c r="B188" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" s="15"/>
       <c r="B189" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" s="15"/>
       <c r="B190" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" s="15"/>
       <c r="B191" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" s="15"/>
       <c r="B192" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" s="15"/>
       <c r="B193" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" s="15"/>
       <c r="B194" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" s="15"/>
       <c r="B195" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" s="15"/>
       <c r="B196" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" s="15"/>
       <c r="B197" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" s="16"/>
       <c r="B198" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -3357,67 +3357,67 @@
         <v>26</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" s="12"/>
       <c r="B200" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" s="12"/>
       <c r="B201" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" s="12"/>
       <c r="B202" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" s="12"/>
       <c r="B203" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" s="12"/>
       <c r="B204" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" s="12"/>
       <c r="B205" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" s="12"/>
       <c r="B206" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" s="12"/>
       <c r="B207" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="12"/>
       <c r="B208" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" s="12"/>
       <c r="B209" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -3453,8 +3453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE9C029-4B67-BC48-953D-ADD0B2B7E79D}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3466,10 +3466,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18">
       <c r="A1" s="17" t="s">
+        <v>304</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>305</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18">
@@ -3487,7 +3487,7 @@
         <v>63</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -3532,7 +3532,7 @@
     </row>
     <row r="8" spans="1:5" ht="18">
       <c r="A8" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B8" s="7"/>
       <c r="D8" s="11"/>
@@ -3553,7 +3553,7 @@
         <v>68</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -3580,17 +3580,17 @@
     </row>
     <row r="13" spans="1:5" ht="17">
       <c r="A13" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" ht="18">
       <c r="A14" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B14" s="6"/>
       <c r="D14" s="11"/>
@@ -3598,7 +3598,7 @@
     </row>
     <row r="15" spans="1:5" ht="17">
       <c r="A15" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B15" s="6"/>
       <c r="D15" s="11"/>
@@ -3609,14 +3609,14 @@
         <v>60</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" ht="18">
       <c r="A17" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B17" s="6"/>
       <c r="D17" s="11"/>
@@ -3624,7 +3624,7 @@
     </row>
     <row r="18" spans="1:5" ht="18">
       <c r="A18" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B18" s="6"/>
       <c r="D18" s="11"/>
@@ -3632,7 +3632,7 @@
     </row>
     <row r="19" spans="1:5" ht="18">
       <c r="A19" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B19" s="6"/>
       <c r="D19" s="11"/>
@@ -3640,7 +3640,7 @@
     </row>
     <row r="20" spans="1:5" ht="18">
       <c r="A20" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B20" s="6"/>
       <c r="D20" s="10"/>
@@ -3648,7 +3648,7 @@
     </row>
     <row r="21" spans="1:5" ht="18">
       <c r="A21" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B21" s="6"/>
       <c r="D21" s="11"/>
@@ -3656,7 +3656,7 @@
     </row>
     <row r="22" spans="1:5" ht="18">
       <c r="A22" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B22" s="6"/>
       <c r="D22" s="11"/>
@@ -3684,10 +3684,10 @@
     </row>
     <row r="25" spans="1:5" ht="17">
       <c r="A25" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
@@ -3704,10 +3704,10 @@
     </row>
     <row r="27" spans="1:5" ht="18">
       <c r="A27" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
@@ -3724,50 +3724,50 @@
     </row>
     <row r="29" spans="1:5" ht="18">
       <c r="A29" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:5" ht="17">
       <c r="A30" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>86</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
     </row>
     <row r="31" spans="1:5" ht="17">
       <c r="A31" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
     </row>
     <row r="32" spans="1:5" ht="17">
       <c r="A32" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
     </row>
     <row r="33" spans="1:5" ht="17">
       <c r="A33" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
@@ -3794,20 +3794,20 @@
     </row>
     <row r="36" spans="1:5" ht="17">
       <c r="A36" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
     </row>
     <row r="37" spans="1:5" ht="17">
       <c r="A37" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
@@ -3822,26 +3822,26 @@
     </row>
     <row r="39" spans="1:5" ht="17">
       <c r="A39" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="17">
       <c r="A40" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="17">
       <c r="A41" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="18">
@@ -3854,10 +3854,10 @@
     </row>
     <row r="43" spans="1:5" ht="17">
       <c r="A43" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18">
@@ -3892,10 +3892,10 @@
     </row>
     <row r="48" spans="1:5" ht="17">
       <c r="A48" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18">
@@ -3924,26 +3924,26 @@
     </row>
     <row r="52" spans="1:5" ht="17">
       <c r="A52" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="17">
       <c r="A53" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="17">
       <c r="A54" s="9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="17">
@@ -3956,7 +3956,7 @@
     </row>
     <row r="56" spans="1:5" ht="18">
       <c r="A56" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>31</v>
@@ -3972,10 +3972,10 @@
     </row>
     <row r="58" spans="1:5" ht="17">
       <c r="A58" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18">

</xml_diff>